<commit_message>
Added Test Data reader from Excel and Database
</commit_message>
<xml_diff>
--- a/AmazonTests/Amazon.Tests/TestData/InputTestData.xlsx
+++ b/AmazonTests/Amazon.Tests/TestData/InputTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Saurabh Dhingra\source\repos\Learning Selenium\Amazon Application\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Saurabh Dhingra\source\repos\Learning Selenium\AmazonTests\Amazon.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A90D88-A272-46D2-85D1-99EBE26EF407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9707153B-1025-4D10-B5A2-43EA72D02F56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Iphone</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Apple Watch</t>
   </si>
 </sst>
 </file>
@@ -354,14 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -381,6 +385,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>